<commit_message>
Added initial support for logging
</commit_message>
<xml_diff>
--- a/tests/test_protocol_multi_task.xlsx
+++ b/tests/test_protocol_multi_task.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10814"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10911"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jespersamsobirch/OneDrive - SniprBiome/ph-meter-interface/tests/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85E3C443-3C30-7741-97E9-8A5E32A82FA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{436E3D79-ABA2-D748-BFB7-D6FEAC2F0B5F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="14400" windowHeight="15980" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -576,8 +576,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AF8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
-      <selection activeCell="T2" sqref="T2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Begam adding support for PID controller.
</commit_message>
<xml_diff>
--- a/tests/test_protocol_multi_task.xlsx
+++ b/tests/test_protocol_multi_task.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10911"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11011"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jespersamsobirch/OneDrive - SniprBiome/ph-meter-interface/tests/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{436E3D79-ABA2-D748-BFB7-D6FEAC2F0B5F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA191614-9A82-3244-A0DB-D6A0BFDE24F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="14400" windowHeight="15980" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="14400" windowHeight="15800" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -577,7 +577,7 @@
   <dimension ref="A1:AF8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -764,14 +764,6 @@
       <c r="AF3"/>
     </row>
     <row r="4" spans="1:32" x14ac:dyDescent="0.2">
-      <c r="A4" s="4"/>
-      <c r="B4" s="3"/>
-      <c r="C4" s="2"/>
-      <c r="D4" s="6"/>
-      <c r="E4" s="5"/>
-      <c r="F4" s="5"/>
-      <c r="G4" s="1"/>
-      <c r="I4" s="1"/>
       <c r="J4"/>
       <c r="K4"/>
       <c r="L4"/>

</xml_diff>